<commit_message>
Ejercios aleatorio no lineal 2/4
</commit_message>
<xml_diff>
--- a/Ejercicios/Metodos Ejercicios_Dual .xlsx
+++ b/Ejercicios/Metodos Ejercicios_Dual .xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sinna\OneDrive\Escritorio\TAREAS SUPERIORES\7° SEMESTRE\METODOS CUANTITATIVOS PARA LA TOMA DE DESICIONES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Metodos\Ejercicios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DD3B72-3AE6-49CF-BEAD-BFF769BC72D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89213B6-7E42-4688-AFE1-2F8BFEEBE06D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="680" activeTab="7" xr2:uid="{44BC6AC9-8240-47AF-B5A8-E4B4770DFC19}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="680" firstSheet="2" activeTab="8" xr2:uid="{44BC6AC9-8240-47AF-B5A8-E4B4770DFC19}"/>
   </bookViews>
   <sheets>
     <sheet name="Ejercicio 1 Primal" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="105">
   <si>
     <t>Min Z = 4a + b</t>
   </si>
@@ -733,6 +733,9 @@
   </si>
   <si>
     <t>Solucion ilimitadas</t>
+  </si>
+  <si>
+    <t>no tiene criterios</t>
   </si>
 </sst>
 </file>
@@ -893,7 +896,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -970,13 +973,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1294,20 +1303,21 @@
   <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="11" max="11" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1315,12 +1325,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1331,7 +1341,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1342,12 +1352,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="D8">
         <v>4</v>
       </c>
@@ -1361,7 +1371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>9</v>
       </c>
@@ -1377,17 +1387,16 @@
       <c r="G9" t="s">
         <v>11</v>
       </c>
-      <c r="K9" t="s">
-        <v>32</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J9" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="34"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>10</v>
       </c>
@@ -1406,21 +1415,13 @@
       <c r="H10">
         <v>150</v>
       </c>
-      <c r="K10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10">
-        <f>O9+O10+O11</f>
-        <v>150</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="O10" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="34"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>11</v>
       </c>
@@ -1439,21 +1440,13 @@
       <c r="H11">
         <v>80</v>
       </c>
-      <c r="K11" t="s">
-        <v>15</v>
-      </c>
-      <c r="L11">
-        <f>O9+O10+O12</f>
-        <v>80</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O11" s="5">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="34"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>12</v>
       </c>
@@ -1472,14 +1465,13 @@
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="N12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="O12" s="5">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="34"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>13</v>
       </c>
@@ -1495,12 +1487,11 @@
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="N13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O13" s="5">
-        <v>0</v>
-      </c>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="33"/>
+      <c r="O13" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1509,23 +1500,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD90F4FC-37C3-4F01-ADE2-C06B1CC8B74A}">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1533,12 +1524,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1546,7 +1537,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1554,7 +1545,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D8">
         <v>-150</v>
       </c>
@@ -1567,8 +1558,13 @@
       <c r="G8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>9</v>
       </c>
@@ -1584,17 +1580,13 @@
       <c r="G9" t="s">
         <v>11</v>
       </c>
-      <c r="J9" t="s">
-        <v>32</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="34"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>10</v>
       </c>
@@ -1614,20 +1606,14 @@
         <v>4</v>
       </c>
       <c r="J10" t="s">
-        <v>24</v>
-      </c>
-      <c r="K10">
-        <f>N9+N10+N11</f>
-        <v>4</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N10" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="33"/>
+      <c r="N10" s="34"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>11</v>
       </c>
@@ -1646,21 +1632,13 @@
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="J11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K11">
-        <f>N9+N10+N12</f>
-        <v>1</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N11" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="34"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>12</v>
       </c>
@@ -1679,14 +1657,13 @@
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="M12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N12" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="34"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>13</v>
       </c>
@@ -1702,12 +1679,18 @@
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="M13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N13" s="5">
-        <v>0</v>
-      </c>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="34"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="32"/>
+      <c r="N14" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1718,31 +1701,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0293216E-2363-478A-A637-1CA512CBF315}">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1753,7 +1736,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1764,7 +1747,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1775,12 +1758,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D9">
         <v>1</v>
       </c>
@@ -1797,7 +1780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>9</v>
       </c>
@@ -1826,7 +1809,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1862,7 +1845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>11</v>
       </c>
@@ -1898,7 +1881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>47</v>
       </c>
@@ -1934,7 +1917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>12</v>
       </c>
@@ -1963,7 +1946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>13</v>
       </c>
@@ -1989,7 +1972,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="D16" s="1">
         <f>D15/D11</f>
         <v>-1</v>
@@ -2011,7 +1994,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>21</v>
       </c>
@@ -2040,7 +2023,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>11</v>
       </c>
@@ -2069,7 +2052,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
         <v>47</v>
       </c>
@@ -2098,7 +2081,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>12</v>
       </c>
@@ -2127,7 +2110,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>13</v>
       </c>
@@ -2152,7 +2135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
       <c r="D23" t="e">
         <f>D22/D20</f>
         <v>#DIV/0!</v>
@@ -2174,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>21</v>
       </c>
@@ -2203,7 +2186,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>11</v>
       </c>
@@ -2232,7 +2215,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>22</v>
       </c>
@@ -2261,7 +2244,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>12</v>
       </c>
@@ -2290,7 +2273,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C29" t="s">
         <v>13</v>
       </c>
@@ -2324,26 +2307,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17931589-CFC8-400E-B042-99ED250EF6F5}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -2351,7 +2334,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>51</v>
       </c>
@@ -2359,12 +2342,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E8">
         <v>10</v>
       </c>
@@ -2381,7 +2364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
         <v>9</v>
       </c>
@@ -2410,7 +2393,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D10" s="1" t="s">
         <v>10</v>
       </c>
@@ -2450,7 +2433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
         <v>11</v>
       </c>
@@ -2486,7 +2469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
         <v>12</v>
       </c>
@@ -2515,7 +2498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>13</v>
       </c>
@@ -2550,7 +2533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="P14" s="4" t="s">
         <v>29</v>
       </c>
@@ -2558,7 +2541,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D15" t="s">
         <v>44</v>
       </c>
@@ -2591,7 +2574,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
@@ -2624,7 +2607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>12</v>
       </c>
@@ -2653,7 +2636,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D18" t="s">
         <v>13</v>
       </c>
@@ -2678,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D20" t="s">
         <v>44</v>
       </c>
@@ -2707,7 +2690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D21" t="s">
         <v>46</v>
       </c>
@@ -2736,7 +2719,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
         <v>12</v>
       </c>
@@ -2765,7 +2748,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>13</v>
       </c>
@@ -2799,28 +2782,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289A2A47-104A-4909-ABA1-76207C3E03C4}">
   <dimension ref="A1:P22"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView topLeftCell="C8" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -2828,7 +2811,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -2836,7 +2819,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -2844,12 +2827,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D9">
         <v>0.1</v>
       </c>
@@ -2875,7 +2858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>9</v>
       </c>
@@ -2908,7 +2891,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
@@ -2948,7 +2931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>11</v>
       </c>
@@ -2988,7 +2971,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>47</v>
       </c>
@@ -3021,7 +3004,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>12</v>
       </c>
@@ -3050,7 +3033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>13</v>
       </c>
@@ -3075,7 +3058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
         <v>22</v>
       </c>
@@ -3104,7 +3087,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>11</v>
       </c>
@@ -3133,7 +3116,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>47</v>
       </c>
@@ -3162,7 +3145,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>12</v>
       </c>
@@ -3191,7 +3174,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>13</v>
       </c>
@@ -3217,7 +3200,7 @@
       </c>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
     </row>
@@ -3230,34 +3213,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B75907-A3E8-4450-A527-F74193C51521}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.44140625" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J4" t="s">
         <v>32</v>
       </c>
@@ -3268,7 +3251,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>69</v>
       </c>
@@ -3289,7 +3272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -3310,7 +3293,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -3321,7 +3304,7 @@
         <v>0.5714285714285714</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="16"/>
       <c r="C8" s="16">
         <v>30</v>
@@ -3346,7 +3329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="16" t="s">
         <v>68</v>
       </c>
@@ -3375,7 +3358,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" s="16" t="s">
         <v>10</v>
       </c>
@@ -3400,7 +3383,7 @@
       </c>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" s="16" t="s">
         <v>11</v>
       </c>
@@ -3425,7 +3408,7 @@
       </c>
       <c r="I11" s="19"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" s="16" t="s">
         <v>12</v>
       </c>
@@ -3448,7 +3431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" s="16" t="s">
         <v>13</v>
       </c>
@@ -3474,7 +3457,7 @@
       </c>
       <c r="H13" s="16"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" s="16"/>
       <c r="C14" s="20">
         <f>C13/C11</f>
@@ -3498,7 +3481,7 @@
       </c>
       <c r="H14" s="16"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
@@ -3507,7 +3490,7 @@
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" s="16" t="s">
         <v>10</v>
       </c>
@@ -3539,7 +3522,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="16" t="s">
         <v>44</v>
       </c>
@@ -3568,7 +3551,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="16" t="s">
         <v>12</v>
       </c>
@@ -3597,7 +3580,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="16" t="s">
         <v>13</v>
       </c>
@@ -3623,14 +3606,14 @@
       </c>
       <c r="H19" s="16"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="12"/>
       <c r="G20" s="12"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="13"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
@@ -3639,7 +3622,7 @@
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="13"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
@@ -3648,7 +3631,7 @@
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="13"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
@@ -3657,7 +3640,7 @@
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="13"/>
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
@@ -3666,11 +3649,11 @@
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="12"/>
       <c r="H26" s="12"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="13"/>
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
@@ -3679,7 +3662,7 @@
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="13"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
@@ -3688,7 +3671,7 @@
       <c r="G29" s="12"/>
       <c r="H29" s="12"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="13"/>
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
@@ -3697,7 +3680,7 @@
       <c r="G30" s="12"/>
       <c r="H30" s="12"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="13"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
@@ -3706,7 +3689,7 @@
       <c r="G31" s="12"/>
       <c r="H31" s="12"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" s="12"/>
     </row>
   </sheetData>
@@ -3719,28 +3702,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A9C6502-CA2F-4FCB-8EBF-73BB700D9A64}">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.109375" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>77</v>
       </c>
@@ -3751,7 +3734,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>78</v>
       </c>
@@ -3762,7 +3745,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -3773,12 +3756,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C9" s="25"/>
       <c r="D9" s="25">
         <v>1</v>
@@ -3799,7 +3782,7 @@
       <c r="O9" s="30"/>
       <c r="P9" s="31"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C10" s="25" t="s">
         <v>9</v>
       </c>
@@ -3824,7 +3807,7 @@
       <c r="O10" s="30"/>
       <c r="P10" s="31"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C11" s="25" t="s">
         <v>10</v>
       </c>
@@ -3849,7 +3832,7 @@
       <c r="O11" s="30"/>
       <c r="P11" s="31"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C12" s="25" t="s">
         <v>11</v>
       </c>
@@ -3874,7 +3857,7 @@
       <c r="O12" s="30"/>
       <c r="P12" s="31"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C13" s="25" t="s">
         <v>47</v>
       </c>
@@ -3899,7 +3882,7 @@
       <c r="O13" s="30"/>
       <c r="P13" s="31"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C14" s="25" t="s">
         <v>12</v>
       </c>
@@ -3924,7 +3907,7 @@
       <c r="O14" s="30"/>
       <c r="P14" s="31"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C15" s="25" t="s">
         <v>13</v>
       </c>
@@ -3949,10 +3932,8 @@
         <v>0</v>
       </c>
       <c r="I15" s="25"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C16" s="25"/>
       <c r="D16" s="25">
         <f>D15/D13</f>
@@ -3976,7 +3957,7 @@
       </c>
       <c r="I16" s="25"/>
     </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C18" s="25" t="s">
         <v>10</v>
       </c>
@@ -4005,7 +3986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C19" s="26" t="s">
         <v>11</v>
       </c>
@@ -4037,7 +4018,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C20" s="25" t="s">
         <v>92</v>
       </c>
@@ -4066,7 +4047,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C21" s="25" t="s">
         <v>12</v>
       </c>
@@ -4095,7 +4076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:11" x14ac:dyDescent="0.3">
       <c r="C22" s="25" t="s">
         <v>13</v>
       </c>
@@ -4121,7 +4102,7 @@
       </c>
       <c r="I22" s="25"/>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:11" x14ac:dyDescent="0.3">
       <c r="D23" s="12">
         <f>D22/D19</f>
         <v>0.33333333333333331</v>
@@ -4152,30 +4133,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAC29BE0-32C7-4E36-A947-5E75DBCC20A5}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="18.600000000000001" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -4183,7 +4164,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -4191,12 +4172,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" s="18"/>
       <c r="C8" s="18">
         <v>-14</v>
@@ -4215,7 +4196,7 @@
       </c>
       <c r="H8" s="18"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="s">
         <v>68</v>
       </c>
@@ -4238,7 +4219,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" s="18" t="s">
         <v>10</v>
       </c>
@@ -4265,7 +4246,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="18" t="s">
         <v>11</v>
       </c>
@@ -4292,7 +4273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" s="18" t="s">
         <v>12</v>
       </c>
@@ -4315,7 +4296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="s">
         <v>13</v>
       </c>
@@ -4341,7 +4322,7 @@
       </c>
       <c r="H13" s="18"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="28"/>
       <c r="C14" s="28"/>
       <c r="D14" s="28"/>
@@ -4350,7 +4331,7 @@
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="18" t="s">
         <v>10</v>
       </c>
@@ -4386,7 +4367,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
         <v>46</v>
       </c>
@@ -4419,7 +4400,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="18" t="s">
         <v>12</v>
       </c>
@@ -4448,7 +4429,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="18" t="s">
         <v>13</v>
       </c>
@@ -4483,21 +4464,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{826AF3CE-33C2-473C-B345-A6840A007703}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>95</v>
       </c>
@@ -4505,32 +4486,32 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>100</v>
       </c>

</xml_diff>